<commit_message>
unifing database to single database.
</commit_message>
<xml_diff>
--- a/AprajitaRetails/Docs/ProjectStatus.xlsx
+++ b/AprajitaRetails/Docs/ProjectStatus.xlsx
@@ -1,18 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Amit Kumar\source\repos\AprajitaRetails\AprajitaRetails\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amitn\Documents\GitHub\AprajitaRetails_Core3.1\AprajitaRetails\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0C714C5-F286-421F-B71C-AC938EFB93AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="119">
   <si>
     <t>Area</t>
   </si>
@@ -138,13 +140,256 @@
   </si>
   <si>
     <t>done</t>
+  </si>
+  <si>
+    <t>Table Name</t>
+  </si>
+  <si>
+    <t>DB Name</t>
+  </si>
+  <si>
+    <t>StoreLocation</t>
+  </si>
+  <si>
+    <t>DailySales</t>
+  </si>
+  <si>
+    <t>DueList</t>
+  </si>
+  <si>
+    <t>DueRecovery</t>
+  </si>
+  <si>
+    <t>CashInHand</t>
+  </si>
+  <si>
+    <t>CashInBank</t>
+  </si>
+  <si>
+    <t>PettyCashExpenses</t>
+  </si>
+  <si>
+    <t>CashExpenes</t>
+  </si>
+  <si>
+    <t>Employee</t>
+  </si>
+  <si>
+    <t>Attendance</t>
+  </si>
+  <si>
+    <t>CurrentSalary</t>
+  </si>
+  <si>
+    <t>Adv Payment</t>
+  </si>
+  <si>
+    <t>Adv Reciept</t>
+  </si>
+  <si>
+    <t>PaySlip</t>
+  </si>
+  <si>
+    <t>Tailoring Booking</t>
+  </si>
+  <si>
+    <t>Tailoring Delivery</t>
+  </si>
+  <si>
+    <t>AprajitaRetailsDB</t>
+  </si>
+  <si>
+    <t>Payments</t>
+  </si>
+  <si>
+    <t>Reciepts</t>
+  </si>
+  <si>
+    <t>CreditNote</t>
+  </si>
+  <si>
+    <t>DebitNotes</t>
+  </si>
+  <si>
+    <t>Party</t>
+  </si>
+  <si>
+    <t>LedgerEntries</t>
+  </si>
+  <si>
+    <t>LedgerMaster</t>
+  </si>
+  <si>
+    <t>LedgerType</t>
+  </si>
+  <si>
+    <t>Bank</t>
+  </si>
+  <si>
+    <t>Accounts</t>
+  </si>
+  <si>
+    <t>Bank Accounts</t>
+  </si>
+  <si>
+    <t>SecurityInfo</t>
+  </si>
+  <si>
+    <t>Bank Deposit</t>
+  </si>
+  <si>
+    <t>Bank Widthwal</t>
+  </si>
+  <si>
+    <t>Cheques Log</t>
+  </si>
+  <si>
+    <t>Store</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>DebitNote</t>
+  </si>
+  <si>
+    <t>ArvindPayments</t>
+  </si>
+  <si>
+    <t>ArvindLedger</t>
+  </si>
+  <si>
+    <t>MaualInvoice</t>
+  </si>
+  <si>
+    <t>Manual InvoiceAdjustmen</t>
+  </si>
+  <si>
+    <t>CashPayments</t>
+  </si>
+  <si>
+    <t>TranscationModes</t>
+  </si>
+  <si>
+    <t>Suspenses</t>
+  </si>
+  <si>
+    <t>EndOfDays</t>
+  </si>
+  <si>
+    <t>MonthEnds</t>
+  </si>
+  <si>
+    <t>IncomeExpensesReport</t>
+  </si>
+  <si>
+    <t>Contact</t>
+  </si>
+  <si>
+    <t>TelegramAuthUsers</t>
+  </si>
+  <si>
+    <t>ToDoMessages</t>
+  </si>
+  <si>
+    <t>CashDetail</t>
+  </si>
+  <si>
+    <t>OnlineSale</t>
+  </si>
+  <si>
+    <t>OnlineVendor</t>
+  </si>
+  <si>
+    <t>AttendancesImport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  ManualSaleItems   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ManualPaymentDetails   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ManualInvoices   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ImportInWard  ImportInWards   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ImportPurchase  ImportPurchases   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ImportSaleItemWise  ImportSaleItemWises   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ImportSaleRegister  ImportSaleRegisters   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ProductItem  ProductItems   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Brand  Brands   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Category  Categories   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Stock  Stocks   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ProductPurchase  ProductPurchases   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Supplier  Suppliers   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PurchaseItem  PurchaseItems   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> PurchaseTaxType  PurchaseTaxTypes   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SalesPerson  SalesPerson   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sales.Models.SaleInvoice  SaleInvoices   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Sales.Models.SaleItem  SaleItems   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SaleTaxType  SaleTaxTypes   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SalePaymentDetail  SalePaymentDetails   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CardPaymentDetail  CardPaymentDetails   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ArvindPayment  ArvindPayments   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RegularInvoice  RegularInvoices   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RegularSaleItem  RegularSaleItems   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RegularPaymentDetail  RegularPaymentDetails   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> RegularCardDetail  RegularCardDetails   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ManualCardDetails   </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -152,16 +397,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -169,14 +426,32 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Input" xfId="1" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -454,10 +729,10 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
@@ -700,4 +975,699 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{652DDEE3-DE94-41D9-9317-4A0AC2FEE136}">
+  <dimension ref="A1:C84"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31:B84"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="48.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="B8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>46</v>
+      </c>
+      <c r="B9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B11" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="B13" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>50</v>
+      </c>
+      <c r="B14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>51</v>
+      </c>
+      <c r="B15" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>52</v>
+      </c>
+      <c r="B16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>54</v>
+      </c>
+      <c r="B18" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>55</v>
+      </c>
+      <c r="B19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>79</v>
+      </c>
+      <c r="B20" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>80</v>
+      </c>
+      <c r="B21" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>81</v>
+      </c>
+      <c r="B22" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>82</v>
+      </c>
+      <c r="B23" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>83</v>
+      </c>
+      <c r="B24" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>84</v>
+      </c>
+      <c r="B25" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>85</v>
+      </c>
+      <c r="B26" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>86</v>
+      </c>
+      <c r="B27" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>87</v>
+      </c>
+      <c r="B28" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>88</v>
+      </c>
+      <c r="B29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>89</v>
+      </c>
+      <c r="B30" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>90</v>
+      </c>
+      <c r="B31" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>57</v>
+      </c>
+      <c r="B32" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>58</v>
+      </c>
+      <c r="B33" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>59</v>
+      </c>
+      <c r="B34" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>60</v>
+      </c>
+      <c r="B35" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>61</v>
+      </c>
+      <c r="B36" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>62</v>
+      </c>
+      <c r="B37" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>63</v>
+      </c>
+      <c r="B38" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>64</v>
+      </c>
+      <c r="B39" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>65</v>
+      </c>
+      <c r="B40" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>66</v>
+      </c>
+      <c r="B41" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>67</v>
+      </c>
+      <c r="B42" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>68</v>
+      </c>
+      <c r="B43" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>69</v>
+      </c>
+      <c r="B44" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>70</v>
+      </c>
+      <c r="B45" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>71</v>
+      </c>
+      <c r="B46" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>72</v>
+      </c>
+      <c r="B47" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>73</v>
+      </c>
+      <c r="B48" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>3</v>
+      </c>
+      <c r="B49" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>14</v>
+      </c>
+      <c r="B50" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>74</v>
+      </c>
+      <c r="B51" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>59</v>
+      </c>
+      <c r="B52" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>75</v>
+      </c>
+      <c r="B53" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>76</v>
+      </c>
+      <c r="B54" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>77</v>
+      </c>
+      <c r="B55" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>78</v>
+      </c>
+      <c r="B56" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>91</v>
+      </c>
+      <c r="B57" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>95</v>
+      </c>
+      <c r="B58" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>96</v>
+      </c>
+      <c r="B59" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>97</v>
+      </c>
+      <c r="B60" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>98</v>
+      </c>
+      <c r="B61" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>99</v>
+      </c>
+      <c r="B62" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>100</v>
+      </c>
+      <c r="B63" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>101</v>
+      </c>
+      <c r="B64" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>102</v>
+      </c>
+      <c r="B65" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>103</v>
+      </c>
+      <c r="B66" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>104</v>
+      </c>
+      <c r="B67" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>105</v>
+      </c>
+      <c r="B68" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>106</v>
+      </c>
+      <c r="B69" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>107</v>
+      </c>
+      <c r="B70" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>108</v>
+      </c>
+      <c r="B71" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>109</v>
+      </c>
+      <c r="B72" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>110</v>
+      </c>
+      <c r="B73" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
+        <v>111</v>
+      </c>
+      <c r="B74" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
+        <v>112</v>
+      </c>
+      <c r="B75" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>113</v>
+      </c>
+      <c r="B76" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
+        <v>114</v>
+      </c>
+      <c r="B77" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>115</v>
+      </c>
+      <c r="B78" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>116</v>
+      </c>
+      <c r="B79" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>117</v>
+      </c>
+      <c r="B80" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>94</v>
+      </c>
+      <c r="B81" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>92</v>
+      </c>
+      <c r="B82" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>93</v>
+      </c>
+      <c r="B83" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>118</v>
+      </c>
+      <c r="B84" t="s">
+        <v>56</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
data mover for adv payment added
</commit_message>
<xml_diff>
--- a/AprajitaRetails/Docs/ProjectStatus.xlsx
+++ b/AprajitaRetails/Docs/ProjectStatus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\amitn\Documents\GitHub\AprajitaRetails_Core3.1\AprajitaRetails\Docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{713692A9-CB31-477F-9F27-194A4D534673}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0498A6CE-C100-46D1-B0DE-CD3F455C173C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1116" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1122" uniqueCount="212">
   <si>
     <t>Area</t>
   </si>
@@ -655,6 +655,18 @@
   </si>
   <si>
     <t>Regular Bill</t>
+  </si>
+  <si>
+    <t>UserId Disabling</t>
+  </si>
+  <si>
+    <t>User id blocking</t>
+  </si>
+  <si>
+    <t>role removing</t>
+  </si>
+  <si>
+    <t>Working for Add and Delete</t>
   </si>
 </sst>
 </file>
@@ -1032,10 +1044,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D45"/>
+  <dimension ref="A1:D48"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1117,7 +1129,7 @@
         <v>11</v>
       </c>
       <c r="D9" t="s">
-        <v>200</v>
+        <v>211</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
@@ -1349,6 +1361,30 @@
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>202</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B46" t="s">
+        <v>208</v>
+      </c>
+      <c r="C46" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B47" t="s">
+        <v>209</v>
+      </c>
+      <c r="C47" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B48" t="s">
+        <v>210</v>
+      </c>
+      <c r="C48" t="s">
+        <v>203</v>
       </c>
     </row>
   </sheetData>

</xml_diff>